<commit_message>
Updated to include three new health datasets
Diabetes, Depression, Coronary Heart Disease
</commit_message>
<xml_diff>
--- a/scripts/Data sources.xlsx
+++ b/scripts/Data sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lambeth.sharepoint.com/sites/StateoftheBorough/Shared Documents/General/Working folder 2023/State of the Borough - flexEdition/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1411" documentId="13_ncr:1_{770093B1-AED3-49DB-9954-741B278843BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{826AB93C-2A15-49A6-9B33-CFC26B2D853B}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="13_ncr:1_{B0CC0253-54B3-4021-92F4-48FB26A7D2A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F17D3D51-2552-4C57-911A-99CDDC2A3415}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" tabRatio="470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="406">
   <si>
     <t>Number</t>
   </si>
@@ -679,9 +679,6 @@
     <t>https://fingertips.phe.org.uk/physical-activity#page/4/gid/1938133001/pat/15/par/E92000001/ati/402/are/E09000022/iid/219/age/1/sex/4/cat/-1/ctp/-1/yrr/1/cid/4/tbm/1/page-options/car-do-0</t>
   </si>
   <si>
-    <t>The percentage of patients with established hypertension, as recorded on practice disease registers (proportion of total list size).</t>
-  </si>
-  <si>
     <t>The graph shows the percentage of patients with established hypertension, as recorded on practice disease registers (proportion of total list size) from 2013 to 2022. No data is available for London. Lambeth has had a lower prevalence than England, and currently has a prevalence of 9%.</t>
   </si>
   <si>
@@ -1252,13 +1249,85 @@
     <t xml:space="preserve">Lambeth 2030 sets out the vision for Lambeth to be a clean, vibrant and lifelong borough, where people can feel safe, have the best conditions to grow up and age well, and live healthier, happier lives.  
 We know Lambeth is a borough of great diversity; our history has been shaped by radicals and reformers, and for hundreds of years, Lambeth has welcomed people from all around the world – providing sanctuary and a place they can call home. 
 We know that residents want to feel proud of their neighbourhoods, building on the strong sense of community across the borough. Residents are concerned with cleanliness and waste, crime and safety, and having accessible parks and open spaces to connect with one another. Residents also want to feel satisfied with the way the Council operates, being communicated with effectively and seeing value for money. </t>
+  </si>
+  <si>
+    <t>The Health and Wellbeing section of State of the Borough report summarises the health of people living Lambeth by bringing together Office for Health Improvement and Dipartites (OHID) data and knowledge with information from other sources to give a broad picture of the health of people in Lambeth today.
+Starting Well
+Setting the foundations for health and wellbeing during pregnancy and in the early years is crucial to ensure we give every child the very best start in life as possible as what happens in pregnancy and early childhood impacts on physical and emotional health all the way through to adulthood. Several outcomes are described in this section:
+•	Childhood vaccinations, MMR dose 1 at age 2 years old
+•	Healthy weight at reception
+•	Good level of development at end of reception
+•	Healthy weight a year 6
+Living well
+Living well is essential in helping us manage our health and maintain our independence.  Unhealthy lifestyle behaviours, such as smoking or drinking alcohol, determine the burden of disease and illness within a population. Many of the risk factors associated with poor health are avoidable and can be prevented in some way by adopting healthy lifestyles. Several outcomes are described in this section:
+•	Wellbeing
+•	Sexual health
+•	Substance misuse
+•	Physical exercise
+•	Healthy weight
+•	Smoking
+•	High blood pressure
+•	Long term conditions
+Aging well
+Over the next 10 years the number of people aged over 50 will grow by 50%. The public health agenda aims to improve the health of our population to enable more years spent in good health. Several outcomes are described in this section:
+•	Life expectancy at birth
+•	Healthy life expectancy
+•	Deaths under 75, preventable cause
+•	Preventable mortality – Covid-19
+•	Preventable mortality – Cancer
+•	Preventable mortality – Cardiovascular disease
+•	Preventable mortality – Liver Disease
+•	Preventable mortality – Respiratory disease
+More detailed information on Health and Wellbeing in Lambeth is available from a range of sources including:
+-	Lambeth JSNA (include weblink)
+-	Health and wellbeing strategy (include weblink)
+-	Health and Care Plan (include weblink) This section has a focus on starting well, living well and aging well in Lambeth, London and England.</t>
+  </si>
+  <si>
+    <t>Diabetes</t>
+  </si>
+  <si>
+    <t>Depression</t>
+  </si>
+  <si>
+    <t>Coronary Heart Disease</t>
+  </si>
+  <si>
+    <t>https://fingertips.phe.org.uk/search/Diabetes#page/4/gid/1/pat/6/par/E12000007/ati/402/are/E09000022/iid/241/age/187/sex/4/cat/-1/ctp/-1/yrr/1/cid/4/tbm/1/page-options/car-do-0</t>
+  </si>
+  <si>
+    <t>https://fingertips.phe.org.uk/search/depression#page/4/gid/1/pat/6/par/E12000007/ati/402/are/E09000022/iid/848/age/168/sex/4/cat/-1/ctp/-1/yrr/1/cid/4/tbm/1/page-options/car-do-0</t>
+  </si>
+  <si>
+    <t>https://fingertips.phe.org.uk/search/chd#page/4/gid/1/pat/6/ati/402/are/E09000022/iid/273/age/1/sex/4/cat/-1/ctp/-1/yrr/1/cid/4/tbm/1</t>
+  </si>
+  <si>
+    <t>The graph shows the percentage of patients aged 17 or over with diabetes mellitus, as recorded on practice disease registers from 2012 to 2022. Lambeth (5.5%) is below the London (6.8%) and national average (7.3%), but has followed the overall increasing trend for 2012 to 2016. Lambeth has leveled off from 2016 to 2022 at around its current value.</t>
+  </si>
+  <si>
+    <t>The graph shows the estimated number of people with depression recorded on the practice register as a proportion of the practice list size, aged 18 years or over, allocated to a local authority boundary using the postcode of the practice from 2009 to 2022. Data for 2009 to 2013 is not available for Lambeth nor London. Across all three regions, the rates of depression has almost doubled since 2013. Lambeth is at 10%, which is greater than London (9.0%) and less than England (13%).</t>
+  </si>
+  <si>
+    <t>The graph shows the percentage of patients with coronary heart disease (CHD), as recorded on practice disease register from 2009 to 2022. Data for 2009 to 2012 is not available for Lambeth nor London. Lambeth (1.2%) has lower rates than London (1.9%) and England (3.0%). All three regions have exhibited a slow and steady decline in CHD rates since 2012.</t>
+  </si>
+  <si>
+    <t>The percentage of patients with established hypertension, as recorded on practice disease registers (proportion of total list size)</t>
+  </si>
+  <si>
+    <t>The percentage of patients aged 17 or over with diabetes mellitus, as recorded on practice disease registers</t>
+  </si>
+  <si>
+    <t>the estimated number of people with depression recorded on the practice register as a proportion of the practice list size, aged 18 years or over, allocated to a local authority boundary using the postcode of the practice</t>
+  </si>
+  <si>
+    <t>The percentage of patients with coronary heart disease (CHD), as recorded on practice disease register</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1316,6 +1385,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF212529"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1359,7 +1434,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1430,6 +1505,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1711,31 +1790,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M105"/>
+  <dimension ref="A1:M108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G94" zoomScale="78" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J97" sqref="J97"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="78" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="8"/>
-    <col min="2" max="2" width="17.1796875" style="7" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="8"/>
+    <col min="2" max="2" width="17.140625" style="7" customWidth="1"/>
     <col min="3" max="3" width="29" style="9" customWidth="1"/>
-    <col min="4" max="4" width="9.1796875" style="10" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" style="7" customWidth="1"/>
-    <col min="6" max="6" width="11.1796875" style="10" customWidth="1"/>
-    <col min="7" max="7" width="28.1796875" style="10" customWidth="1"/>
-    <col min="8" max="8" width="34.81640625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="19.1796875" style="7" customWidth="1"/>
-    <col min="10" max="10" width="17.1796875" style="7" customWidth="1"/>
-    <col min="11" max="11" width="97.1796875" style="7" customWidth="1"/>
-    <col min="12" max="12" width="59.54296875" style="10" customWidth="1"/>
-    <col min="13" max="13" width="29.81640625" style="10" customWidth="1"/>
-    <col min="14" max="16384" width="8.81640625" style="10"/>
+    <col min="4" max="4" width="9.140625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="28.140625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="34.85546875" style="7" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="17.140625" style="7" customWidth="1"/>
+    <col min="11" max="11" width="97.140625" style="7" customWidth="1"/>
+    <col min="12" max="12" width="59.5703125" style="10" customWidth="1"/>
+    <col min="13" max="13" width="29.85546875" style="10" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1773,7 +1852,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>0</v>
       </c>
@@ -1787,7 +1866,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="13"/>
       <c r="I2" s="7" t="str">
-        <f t="shared" ref="I2:I63" si="0">LOWER(SUBSTITUTE(C2," ","-"))</f>
+        <f t="shared" ref="I2:I66" si="0">LOWER(SUBSTITUTE(C2," ","-"))</f>
         <v>introduction</v>
       </c>
       <c r="J2" s="7" t="str">
@@ -1798,7 +1877,7 @@
       <c r="L2" s="13"/>
       <c r="M2" s="13"/>
     </row>
-    <row r="3" spans="1:13" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>1</v>
       </c>
@@ -1823,7 +1902,7 @@
       <c r="L3" s="13"/>
       <c r="M3" s="13"/>
     </row>
-    <row r="4" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>2</v>
       </c>
@@ -1860,7 +1939,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>3</v>
       </c>
@@ -1894,7 +1973,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>4</v>
       </c>
@@ -1928,7 +2007,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>5</v>
       </c>
@@ -1962,7 +2041,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>6</v>
       </c>
@@ -1996,7 +2075,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>7</v>
       </c>
@@ -2030,7 +2109,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>8</v>
       </c>
@@ -2064,7 +2143,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>9</v>
       </c>
@@ -2098,7 +2177,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>10</v>
       </c>
@@ -2132,7 +2211,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="116" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>11</v>
       </c>
@@ -2166,7 +2245,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>12</v>
       </c>
@@ -2183,7 +2262,7 @@
         <v>#jobs-earnings-and-businesses-introduction</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>13</v>
       </c>
@@ -2220,7 +2299,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="145" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>14</v>
       </c>
@@ -2257,7 +2336,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="87" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>15</v>
       </c>
@@ -2292,7 +2371,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="87" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>16</v>
       </c>
@@ -2329,7 +2408,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" ht="180" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>17</v>
       </c>
@@ -2366,7 +2445,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>18</v>
       </c>
@@ -2400,7 +2479,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="58" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>19</v>
       </c>
@@ -2437,7 +2516,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>20</v>
       </c>
@@ -2474,7 +2553,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>21</v>
       </c>
@@ -2511,7 +2590,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="87" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>22</v>
       </c>
@@ -2545,7 +2624,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="87" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>23</v>
       </c>
@@ -2582,7 +2661,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="58" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>24</v>
       </c>
@@ -2619,7 +2698,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>25</v>
       </c>
@@ -2637,7 +2716,7 @@
         <v>#financial-resilience-introduction</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <v>26</v>
       </c>
@@ -2671,7 +2750,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>27</v>
       </c>
@@ -2705,7 +2784,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <v>28</v>
       </c>
@@ -2740,7 +2819,7 @@
       </c>
       <c r="L30" s="7"/>
     </row>
-    <row r="31" spans="1:12" ht="87" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>29</v>
       </c>
@@ -2774,7 +2853,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="391.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" ht="405" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>30</v>
       </c>
@@ -2808,7 +2887,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
         <v>31</v>
       </c>
@@ -2826,7 +2905,7 @@
         <v>#education-introduction</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>32</v>
       </c>
@@ -2860,7 +2939,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
         <v>33</v>
       </c>
@@ -2894,7 +2973,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
         <v>34</v>
       </c>
@@ -2928,7 +3007,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
         <v>35</v>
       </c>
@@ -2962,7 +3041,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
         <v>36</v>
       </c>
@@ -2996,7 +3075,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A39" s="8">
         <v>37</v>
       </c>
@@ -3030,7 +3109,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
         <v>38</v>
       </c>
@@ -3064,7 +3143,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="8">
         <v>39</v>
       </c>
@@ -3098,7 +3177,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
         <v>40</v>
       </c>
@@ -3132,7 +3211,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" s="8">
         <v>41</v>
       </c>
@@ -3166,7 +3245,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A44" s="12">
         <v>42</v>
       </c>
@@ -3181,8 +3260,11 @@
         <f t="shared" si="1"/>
         <v>#health-and-wellbeing-introduction</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" s="11" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="K44" s="7" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" s="11" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
         <v>43</v>
       </c>
@@ -3210,14 +3292,14 @@
         <v>childhood-vaccinations</v>
       </c>
       <c r="J45" s="7" t="str">
-        <f t="shared" ref="J45:J104" si="4">_xlfn.CONCAT("#",I45)</f>
+        <f t="shared" ref="J45:J107" si="4">_xlfn.CONCAT("#",I45)</f>
         <v>#childhood-vaccinations</v>
       </c>
       <c r="K45" s="7" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
         <v>44</v>
       </c>
@@ -3251,7 +3333,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="47" spans="1:13" s="1" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
         <v>45</v>
       </c>
@@ -3288,7 +3370,7 @@
       <c r="L47" s="15"/>
       <c r="M47" s="15"/>
     </row>
-    <row r="48" spans="1:13" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" s="12">
         <v>46</v>
       </c>
@@ -3325,7 +3407,7 @@
       <c r="L48" s="15"/>
       <c r="M48" s="15"/>
     </row>
-    <row r="49" spans="1:13" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" ht="195" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
         <v>47</v>
       </c>
@@ -3359,7 +3441,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="12"/>
       <c r="B50" s="7" t="s">
         <v>166</v>
@@ -3391,7 +3473,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="51" spans="1:13" s="1" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" s="8">
         <f>A49+1</f>
         <v>48</v>
@@ -3429,7 +3511,7 @@
       <c r="L51" s="15"/>
       <c r="M51" s="15"/>
     </row>
-    <row r="52" spans="1:13" s="1" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <f>A51+1</f>
         <v>49</v>
@@ -3467,9 +3549,9 @@
       <c r="L52" s="15"/>
       <c r="M52" s="15"/>
     </row>
-    <row r="53" spans="1:13" s="1" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A53" s="8">
-        <f t="shared" ref="A53:A104" si="5">A52+1</f>
+        <f t="shared" ref="A53:A107" si="5">A52+1</f>
         <v>50</v>
       </c>
       <c r="B53" s="7" t="s">
@@ -3505,7 +3587,7 @@
       <c r="L53" s="15"/>
       <c r="M53" s="15"/>
     </row>
-    <row r="54" spans="1:13" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
         <f t="shared" si="5"/>
         <v>51</v>
@@ -3543,7 +3625,7 @@
       <c r="L54" s="15"/>
       <c r="M54" s="15"/>
     </row>
-    <row r="55" spans="1:13" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <f t="shared" si="5"/>
         <v>52</v>
@@ -3565,23 +3647,23 @@
         <v>207</v>
       </c>
       <c r="H55" s="21" t="s">
+        <v>402</v>
+      </c>
+      <c r="I55" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>high-blood-pressure</v>
+      </c>
+      <c r="J55" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>#high-blood-pressure</v>
+      </c>
+      <c r="K55" s="7" t="s">
         <v>208</v>
-      </c>
-      <c r="I55" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>high-blood-pressure</v>
-      </c>
-      <c r="J55" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>#high-blood-pressure</v>
-      </c>
-      <c r="K55" s="7" t="s">
-        <v>209</v>
       </c>
       <c r="L55" s="15"/>
       <c r="M55" s="15"/>
     </row>
-    <row r="56" spans="1:13" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="8">
         <f t="shared" si="5"/>
         <v>53</v>
@@ -3590,21 +3672,21 @@
         <v>166</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D56" s="17">
         <v>2023</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F56" s="15"/>
       <c r="G56" s="16" t="s">
+        <v>381</v>
+      </c>
+      <c r="H56" s="21" t="s">
         <v>382</v>
       </c>
-      <c r="H56" s="21" t="s">
-        <v>383</v>
-      </c>
       <c r="I56" s="7" t="str">
         <f t="shared" si="0"/>
         <v>drug-and-alcohol-misuse</v>
@@ -3614,12 +3696,12 @@
         <v>#drug-and-alcohol-misuse</v>
       </c>
       <c r="K56" s="7" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="L56" s="15"/>
       <c r="M56" s="15"/>
     </row>
-    <row r="57" spans="1:13" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A57" s="8">
         <f t="shared" si="5"/>
         <v>54</v>
@@ -3628,36 +3710,36 @@
         <v>166</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>385</v>
+        <v>393</v>
       </c>
       <c r="D57" s="17">
-        <v>2021</v>
-      </c>
-      <c r="E57" s="7" t="s">
+        <v>2022</v>
+      </c>
+      <c r="E57" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="F57" s="9"/>
-      <c r="G57" s="15" t="s">
-        <v>384</v>
-      </c>
-      <c r="H57" s="21" t="s">
-        <v>386</v>
+      <c r="F57" s="15"/>
+      <c r="G57" s="16" t="s">
+        <v>396</v>
+      </c>
+      <c r="H57" s="25" t="s">
+        <v>403</v>
       </c>
       <c r="I57" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>life-expectancy-at-birth</v>
+        <v>diabetes</v>
       </c>
       <c r="J57" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#life-expectancy-at-birth</v>
+        <v>#diabetes</v>
       </c>
       <c r="K57" s="7" t="s">
-        <v>387</v>
+        <v>399</v>
       </c>
       <c r="L57" s="15"/>
       <c r="M57" s="15"/>
     </row>
-    <row r="58" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:13" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A58" s="8">
         <f t="shared" si="5"/>
         <v>55</v>
@@ -3665,34 +3747,37 @@
       <c r="B58" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="C58" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="D58" s="10">
-        <v>2020</v>
-      </c>
-      <c r="E58" s="7" t="s">
+      <c r="C58" s="15" t="s">
+        <v>394</v>
+      </c>
+      <c r="D58" s="17">
+        <v>2022</v>
+      </c>
+      <c r="E58" s="9" t="s">
         <v>168</v>
       </c>
+      <c r="F58" s="15"/>
       <c r="G58" s="16" t="s">
-        <v>211</v>
-      </c>
-      <c r="H58" s="7" t="s">
-        <v>212</v>
+        <v>397</v>
+      </c>
+      <c r="H58" s="25" t="s">
+        <v>404</v>
       </c>
       <c r="I58" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>healthy-life-expectancy</v>
+        <f t="shared" ref="I58:I59" si="6">LOWER(SUBSTITUTE(C58," ","-"))</f>
+        <v>depression</v>
       </c>
       <c r="J58" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>#healthy-life-expectancy</v>
+        <f t="shared" ref="J58:J59" si="7">_xlfn.CONCAT("#",I58)</f>
+        <v>#depression</v>
       </c>
       <c r="K58" s="7" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>400</v>
+      </c>
+      <c r="L58" s="15"/>
+      <c r="M58" s="15"/>
+    </row>
+    <row r="59" spans="1:13" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" s="8">
         <f t="shared" si="5"/>
         <v>56</v>
@@ -3700,34 +3785,37 @@
       <c r="B59" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="C59" s="9" t="s">
-        <v>390</v>
-      </c>
-      <c r="D59" s="10">
-        <v>2021</v>
-      </c>
-      <c r="E59" s="18" t="s">
+      <c r="C59" s="15" t="s">
+        <v>395</v>
+      </c>
+      <c r="D59" s="17">
+        <v>2022</v>
+      </c>
+      <c r="E59" s="9" t="s">
         <v>168</v>
       </c>
+      <c r="F59" s="15"/>
       <c r="G59" s="16" t="s">
-        <v>214</v>
-      </c>
-      <c r="H59" s="7" t="s">
-        <v>215</v>
+        <v>398</v>
+      </c>
+      <c r="H59" s="25" t="s">
+        <v>405</v>
       </c>
       <c r="I59" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>deaths-under-75-from-preventable-causes</v>
+        <f t="shared" si="6"/>
+        <v>coronary-heart-disease</v>
       </c>
       <c r="J59" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>#deaths-under-75-from-preventable-causes</v>
-      </c>
-      <c r="K59" s="21" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+        <f t="shared" si="7"/>
+        <v>#coronary-heart-disease</v>
+      </c>
+      <c r="K59" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="L59" s="15"/>
+      <c r="M59" s="15"/>
+    </row>
+    <row r="60" spans="1:13" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A60" s="8">
         <f t="shared" si="5"/>
         <v>57</v>
@@ -3735,34 +3823,37 @@
       <c r="B60" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="C60" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="D60" s="10">
-        <v>2023</v>
+      <c r="C60" s="15" t="s">
+        <v>384</v>
+      </c>
+      <c r="D60" s="17">
+        <v>2021</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="G60" s="16" t="s">
-        <v>219</v>
-      </c>
-      <c r="H60" s="7" t="s">
-        <v>220</v>
+        <v>168</v>
+      </c>
+      <c r="F60" s="9"/>
+      <c r="G60" s="15" t="s">
+        <v>383</v>
+      </c>
+      <c r="H60" s="21" t="s">
+        <v>385</v>
       </c>
       <c r="I60" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>covid-deaths-per-capita</v>
+        <v>life-expectancy-at-birth</v>
       </c>
       <c r="J60" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#covid-deaths-per-capita</v>
-      </c>
-      <c r="K60" s="22" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+        <v>#life-expectancy-at-birth</v>
+      </c>
+      <c r="K60" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="L60" s="15"/>
+      <c r="M60" s="15"/>
+    </row>
+    <row r="61" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="8">
         <f t="shared" si="5"/>
         <v>58</v>
@@ -3770,32 +3861,34 @@
       <c r="B61" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="C61" s="15" t="s">
-        <v>222</v>
+      <c r="C61" s="9" t="s">
+        <v>209</v>
       </c>
       <c r="D61" s="10">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E61" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="F61" s="7"/>
       <c r="G61" s="16" t="s">
-        <v>223</v>
+        <v>210</v>
+      </c>
+      <c r="H61" s="7" t="s">
+        <v>211</v>
       </c>
       <c r="I61" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>preventable-mortality---cancer</v>
+        <v>healthy-life-expectancy</v>
       </c>
       <c r="J61" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#preventable-mortality---cancer</v>
-      </c>
-      <c r="K61" s="22" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>#healthy-life-expectancy</v>
+      </c>
+      <c r="K61" s="7" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="8">
         <f t="shared" si="5"/>
         <v>59</v>
@@ -3803,32 +3896,34 @@
       <c r="B62" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="C62" s="15" t="s">
-        <v>225</v>
+      <c r="C62" s="9" t="s">
+        <v>389</v>
       </c>
       <c r="D62" s="10">
         <v>2021</v>
       </c>
-      <c r="E62" s="7" t="s">
+      <c r="E62" s="18" t="s">
         <v>168</v>
       </c>
-      <c r="F62" s="7"/>
       <c r="G62" s="16" t="s">
-        <v>226</v>
+        <v>213</v>
+      </c>
+      <c r="H62" s="7" t="s">
+        <v>214</v>
       </c>
       <c r="I62" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>preventable-mortality---cardiovascular-disease</v>
+        <v>deaths-under-75-from-preventable-causes</v>
       </c>
       <c r="J62" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#preventable-mortality---cardiovascular-disease</v>
-      </c>
-      <c r="K62" s="22" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+        <v>#deaths-under-75-from-preventable-causes</v>
+      </c>
+      <c r="K62" s="21" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="8">
         <f t="shared" si="5"/>
         <v>60</v>
@@ -3836,32 +3931,34 @@
       <c r="B63" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="C63" s="15" t="s">
-        <v>228</v>
+      <c r="C63" s="9" t="s">
+        <v>216</v>
       </c>
       <c r="D63" s="10">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="F63" s="7"/>
+        <v>217</v>
+      </c>
       <c r="G63" s="16" t="s">
-        <v>229</v>
+        <v>218</v>
+      </c>
+      <c r="H63" s="7" t="s">
+        <v>219</v>
       </c>
       <c r="I63" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>preventable-mortality---liver-disease</v>
+        <v>covid-deaths-per-capita</v>
       </c>
       <c r="J63" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#preventable-mortality---liver-disease</v>
+        <v>#covid-deaths-per-capita</v>
       </c>
       <c r="K63" s="22" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="8">
         <f t="shared" si="5"/>
         <v>61</v>
@@ -3870,7 +3967,7 @@
         <v>166</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="D64" s="10">
         <v>2021</v>
@@ -3879,964 +3976,961 @@
         <v>168</v>
       </c>
       <c r="F64" s="7"/>
-      <c r="G64" s="16" t="s">
-        <v>232</v>
+      <c r="G64" s="24" t="s">
+        <v>222</v>
       </c>
       <c r="I64" s="7" t="str">
-        <f t="shared" ref="I64:I104" si="6">LOWER(SUBSTITUTE(C64," ","-"))</f>
-        <v>preventable-mortality---respiratory-disease</v>
+        <f t="shared" si="0"/>
+        <v>preventable-mortality---cancer</v>
       </c>
       <c r="J64" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#preventable-mortality---respiratory-disease</v>
+        <v>#preventable-mortality---cancer</v>
       </c>
       <c r="K64" s="22" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="8">
         <f t="shared" si="5"/>
         <v>62</v>
       </c>
-      <c r="C65" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="G65" s="14"/>
+      <c r="B65" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C65" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="D65" s="10">
+        <v>2021</v>
+      </c>
+      <c r="E65" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F65" s="7"/>
+      <c r="G65" s="24" t="s">
+        <v>225</v>
+      </c>
       <c r="I65" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>crime-safety-and-justice-introduction</v>
+        <f t="shared" si="0"/>
+        <v>preventable-mortality---cardiovascular-disease</v>
       </c>
       <c r="J65" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#crime-safety-and-justice-introduction</v>
-      </c>
-      <c r="K65" s="7" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+        <v>#preventable-mortality---cardiovascular-disease</v>
+      </c>
+      <c r="K65" s="22" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="8">
         <f t="shared" si="5"/>
         <v>63</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="C66" s="9" t="s">
-        <v>237</v>
+        <v>166</v>
+      </c>
+      <c r="C66" s="15" t="s">
+        <v>227</v>
       </c>
       <c r="D66" s="10">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="G66" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="H66" s="7" t="s">
-        <v>240</v>
+        <v>168</v>
+      </c>
+      <c r="F66" s="7"/>
+      <c r="G66" s="24" t="s">
+        <v>228</v>
       </c>
       <c r="I66" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>overall-crime-rate</v>
+        <f t="shared" si="0"/>
+        <v>preventable-mortality---liver-disease</v>
       </c>
       <c r="J66" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#overall-crime-rate</v>
-      </c>
-      <c r="K66" s="7" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+        <v>#preventable-mortality---liver-disease</v>
+      </c>
+      <c r="K66" s="22" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="8">
         <f t="shared" si="5"/>
         <v>64</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="C67" s="9" t="s">
-        <v>242</v>
+        <v>166</v>
+      </c>
+      <c r="C67" s="15" t="s">
+        <v>230</v>
       </c>
       <c r="D67" s="10">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="G67" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="H67" s="7" t="s">
-        <v>243</v>
+        <v>168</v>
+      </c>
+      <c r="F67" s="7"/>
+      <c r="G67" s="24" t="s">
+        <v>231</v>
       </c>
       <c r="I67" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>violent-crime-rate</v>
+        <f t="shared" ref="I67:I107" si="8">LOWER(SUBSTITUTE(C67," ","-"))</f>
+        <v>preventable-mortality---respiratory-disease</v>
       </c>
       <c r="J67" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#violent-crime-rate</v>
-      </c>
-      <c r="K67" s="7" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+        <v>#preventable-mortality---respiratory-disease</v>
+      </c>
+      <c r="K67" s="22" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="8">
         <f t="shared" si="5"/>
         <v>65</v>
       </c>
-      <c r="B68" s="7" t="s">
-        <v>236</v>
-      </c>
       <c r="C68" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="D68" s="10">
-        <v>2022</v>
-      </c>
-      <c r="E68" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="G68" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="H68" s="7" t="s">
-        <v>246</v>
-      </c>
+        <v>233</v>
+      </c>
+      <c r="G68" s="14"/>
       <c r="I68" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>knife-crime-rate</v>
+        <f t="shared" si="8"/>
+        <v>crime-safety-and-justice-introduction</v>
       </c>
       <c r="J68" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#knife-crime-rate</v>
+        <v>#crime-safety-and-justice-introduction</v>
       </c>
       <c r="K68" s="7" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" ht="87" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A69" s="8">
         <f t="shared" si="5"/>
         <v>66</v>
       </c>
       <c r="B69" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="C69" s="9" t="s">
         <v>236</v>
-      </c>
-      <c r="C69" s="9" t="s">
-        <v>248</v>
       </c>
       <c r="D69" s="10">
         <v>2022</v>
       </c>
       <c r="E69" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="G69" s="14" t="s">
         <v>238</v>
       </c>
-      <c r="G69" s="14" t="s">
+      <c r="H69" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="H69" s="7" t="s">
-        <v>249</v>
-      </c>
       <c r="I69" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>knife-crime-rate-with-victims-younger-than-25</v>
+        <f t="shared" si="8"/>
+        <v>overall-crime-rate</v>
       </c>
       <c r="J69" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#knife-crime-rate-with-victims-younger-than-25</v>
+        <v>#overall-crime-rate</v>
       </c>
       <c r="K69" s="7" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A70" s="8">
         <f t="shared" si="5"/>
         <v>67</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="D70" s="10">
         <v>2022</v>
       </c>
       <c r="E70" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="G70" s="14" t="s">
         <v>238</v>
       </c>
-      <c r="G70" s="14" t="s">
-        <v>239</v>
-      </c>
       <c r="H70" s="7" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="I70" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>domestic-abuse-crime-rate</v>
+        <f t="shared" si="8"/>
+        <v>violent-crime-rate</v>
       </c>
       <c r="J70" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#domestic-abuse-crime-rate</v>
+        <v>#violent-crime-rate</v>
       </c>
       <c r="K70" s="7" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" ht="130.5" x14ac:dyDescent="0.35">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A71" s="8">
         <f t="shared" si="5"/>
         <v>68</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="D71" s="10">
         <v>2022</v>
       </c>
       <c r="E71" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="G71" s="14" t="s">
         <v>238</v>
       </c>
-      <c r="G71" s="14" t="s">
-        <v>239</v>
-      </c>
       <c r="H71" s="7" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="I71" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>hate-crime-rate</v>
+        <f t="shared" si="8"/>
+        <v>knife-crime-rate</v>
       </c>
       <c r="J71" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#hate-crime-rate</v>
+        <v>#knife-crime-rate</v>
       </c>
       <c r="K71" s="7" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" ht="116" x14ac:dyDescent="0.35">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A72" s="8">
         <f t="shared" si="5"/>
         <v>69</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="D72" s="10">
         <v>2022</v>
       </c>
       <c r="E72" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="G72" s="14" t="s">
         <v>238</v>
       </c>
-      <c r="G72" s="14" t="s">
-        <v>239</v>
-      </c>
       <c r="H72" s="7" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="I72" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>drug-related-crime-rate</v>
+        <f t="shared" si="8"/>
+        <v>knife-crime-rate-with-victims-younger-than-25</v>
       </c>
       <c r="J72" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#drug-related-crime-rate</v>
+        <v>#knife-crime-rate-with-victims-younger-than-25</v>
       </c>
       <c r="K72" s="7" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" ht="116" x14ac:dyDescent="0.35">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A73" s="8">
         <f t="shared" si="5"/>
         <v>70</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="D73" s="10">
         <v>2022</v>
       </c>
       <c r="E73" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="G73" s="14" t="s">
         <v>238</v>
       </c>
-      <c r="G73" s="14" t="s">
-        <v>239</v>
-      </c>
       <c r="H73" s="7" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="I73" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>domestic-burglary-crime-rate</v>
+        <f t="shared" si="8"/>
+        <v>domestic-abuse-crime-rate</v>
       </c>
       <c r="J73" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#domestic-burglary-crime-rate</v>
+        <v>#domestic-abuse-crime-rate</v>
       </c>
       <c r="K73" s="7" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" ht="87" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A74" s="8">
         <f t="shared" si="5"/>
         <v>71</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="D74" s="10">
         <v>2022</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>264</v>
+        <v>237</v>
       </c>
       <c r="G74" s="14" t="s">
-        <v>265</v>
+        <v>238</v>
       </c>
       <c r="H74" s="7" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="I74" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>anti-social-behaviour</v>
+        <f t="shared" si="8"/>
+        <v>hate-crime-rate</v>
       </c>
       <c r="J74" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#anti-social-behaviour</v>
+        <v>#hate-crime-rate</v>
       </c>
       <c r="K74" s="7" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A75" s="8">
         <f t="shared" si="5"/>
         <v>72</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="D75" s="10">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="E75" s="7" t="s">
-        <v>269</v>
+        <v>237</v>
       </c>
       <c r="G75" s="14" t="s">
-        <v>270</v>
+        <v>238</v>
       </c>
       <c r="H75" s="7" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="I75" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>reoffending-rates</v>
+        <f t="shared" si="8"/>
+        <v>drug-related-crime-rate</v>
       </c>
       <c r="J75" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#reoffending-rates</v>
+        <v>#drug-related-crime-rate</v>
       </c>
       <c r="K75" s="7" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" ht="116" x14ac:dyDescent="0.35">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A76" s="8">
         <f t="shared" si="5"/>
         <v>73</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="D76" s="10">
         <v>2022</v>
       </c>
       <c r="E76" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="G76" s="14" t="s">
         <v>238</v>
       </c>
-      <c r="F76" s="19" t="s">
-        <v>274</v>
-      </c>
-      <c r="G76" s="14" t="s">
-        <v>275</v>
-      </c>
       <c r="H76" s="7" t="s">
-        <v>276</v>
+        <v>260</v>
       </c>
       <c r="I76" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>stop-and-search</v>
+        <f t="shared" si="8"/>
+        <v>domestic-burglary-crime-rate</v>
       </c>
       <c r="J76" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#stop-and-search</v>
+        <v>#domestic-burglary-crime-rate</v>
       </c>
       <c r="K76" s="7" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" s="11" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A77" s="8">
         <f t="shared" si="5"/>
         <v>74</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>278</v>
+        <v>262</v>
       </c>
       <c r="D77" s="10">
         <v>2022</v>
       </c>
       <c r="E77" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="F77" s="10"/>
+        <v>263</v>
+      </c>
       <c r="G77" s="14" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="H77" s="7" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="I77" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>public-perception-of-police</v>
+        <f t="shared" si="8"/>
+        <v>anti-social-behaviour</v>
       </c>
       <c r="J77" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#public-perception-of-police</v>
+        <v>#anti-social-behaviour</v>
       </c>
       <c r="K77" s="7" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" ht="130.5" x14ac:dyDescent="0.35">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A78" s="8">
         <f t="shared" si="5"/>
         <v>75</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="D78" s="10">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="E78" s="7" t="s">
-        <v>102</v>
+        <v>268</v>
       </c>
       <c r="G78" s="14" t="s">
-        <v>103</v>
+        <v>269</v>
       </c>
       <c r="H78" s="7" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="I78" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>resident-survey-perception-of-safety</v>
+        <f t="shared" si="8"/>
+        <v>reoffending-rates</v>
       </c>
       <c r="J78" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#resident-survey-perception-of-safety</v>
+        <v>#reoffending-rates</v>
       </c>
       <c r="K78" s="7" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A79" s="8">
         <f t="shared" si="5"/>
         <v>76</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="D79" s="10">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="E79" s="7" t="s">
-        <v>286</v>
+        <v>237</v>
+      </c>
+      <c r="F79" s="19" t="s">
+        <v>273</v>
       </c>
       <c r="G79" s="14" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
       <c r="H79" s="7" t="s">
-        <v>288</v>
+        <v>275</v>
       </c>
       <c r="I79" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>traffic-incidents</v>
+        <f t="shared" si="8"/>
+        <v>stop-and-search</v>
       </c>
       <c r="J79" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#traffic-incidents</v>
+        <v>#stop-and-search</v>
       </c>
       <c r="K79" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="8">
         <f t="shared" si="5"/>
         <v>77</v>
       </c>
+      <c r="B80" s="7" t="s">
+        <v>235</v>
+      </c>
       <c r="C80" s="9" t="s">
-        <v>290</v>
-      </c>
-      <c r="G80" s="14"/>
+        <v>277</v>
+      </c>
+      <c r="D80" s="10">
+        <v>2022</v>
+      </c>
+      <c r="E80" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="F80" s="10"/>
+      <c r="G80" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="H80" s="7" t="s">
+        <v>279</v>
+      </c>
       <c r="I80" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>environment-introduction</v>
+        <f t="shared" si="8"/>
+        <v>public-perception-of-police</v>
       </c>
       <c r="J80" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#environment-introduction</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+        <v>#public-perception-of-police</v>
+      </c>
+      <c r="K80" s="7" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A81" s="8">
         <f t="shared" si="5"/>
         <v>78</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>291</v>
+        <v>235</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="D81" s="10">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="E81" s="7" t="s">
-        <v>293</v>
+        <v>102</v>
       </c>
       <c r="G81" s="14" t="s">
-        <v>294</v>
+        <v>103</v>
       </c>
       <c r="H81" s="7" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
       <c r="I81" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>greenhouse-gas-emissions</v>
+        <f t="shared" si="8"/>
+        <v>resident-survey-perception-of-safety</v>
       </c>
       <c r="J81" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#greenhouse-gas-emissions</v>
+        <v>#resident-survey-perception-of-safety</v>
       </c>
       <c r="K81" s="7" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" ht="174" x14ac:dyDescent="0.35">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" s="8">
         <f t="shared" si="5"/>
         <v>79</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>291</v>
+        <v>235</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="D82" s="10">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="E82" s="7" t="s">
-        <v>298</v>
-      </c>
-      <c r="G82" s="10" t="s">
-        <v>299</v>
+        <v>285</v>
+      </c>
+      <c r="G82" s="14" t="s">
+        <v>286</v>
       </c>
       <c r="H82" s="7" t="s">
-        <v>300</v>
+        <v>287</v>
       </c>
       <c r="I82" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>pollutant-concentrations</v>
+        <f t="shared" si="8"/>
+        <v>traffic-incidents</v>
       </c>
       <c r="J82" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#pollutant-concentrations</v>
+        <v>#traffic-incidents</v>
       </c>
       <c r="K82" s="7" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="8">
         <f t="shared" si="5"/>
         <v>80</v>
       </c>
-      <c r="B83" s="7" t="s">
-        <v>291</v>
-      </c>
       <c r="C83" s="9" t="s">
-        <v>302</v>
-      </c>
-      <c r="D83" s="10">
-        <v>2021</v>
-      </c>
-      <c r="E83" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="G83" s="14" t="s">
-        <v>304</v>
-      </c>
-      <c r="H83" s="7" t="s">
-        <v>305</v>
-      </c>
+        <v>289</v>
+      </c>
+      <c r="G83" s="14"/>
       <c r="I83" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>recycling-rates</v>
+        <f t="shared" si="8"/>
+        <v>environment-introduction</v>
       </c>
       <c r="J83" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#recycling-rates</v>
-      </c>
-      <c r="K83" s="7" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+        <v>#environment-introduction</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A84" s="8">
         <f t="shared" si="5"/>
         <v>81</v>
       </c>
       <c r="B84" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="C84" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="C84" s="9" t="s">
-        <v>307</v>
-      </c>
       <c r="D84" s="10">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="E84" s="7" t="s">
-        <v>308</v>
-      </c>
-      <c r="G84" s="10" t="s">
-        <v>309</v>
+        <v>292</v>
+      </c>
+      <c r="G84" s="14" t="s">
+        <v>293</v>
       </c>
       <c r="H84" s="7" t="s">
-        <v>310</v>
+        <v>294</v>
       </c>
       <c r="I84" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>energy-performance-certificate-ratings</v>
+        <f t="shared" si="8"/>
+        <v>greenhouse-gas-emissions</v>
       </c>
       <c r="J84" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#energy-performance-certificate-ratings</v>
+        <v>#greenhouse-gas-emissions</v>
       </c>
       <c r="K84" s="7" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" ht="180" x14ac:dyDescent="0.25">
       <c r="A85" s="8">
         <f t="shared" si="5"/>
         <v>82</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
       <c r="D85" s="10">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="E85" s="7" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="G85" s="10" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
       <c r="H85" s="7" t="s">
-        <v>314</v>
+        <v>299</v>
       </c>
       <c r="I85" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>solar-panel-installations</v>
+        <f t="shared" si="8"/>
+        <v>pollutant-concentrations</v>
       </c>
       <c r="J85" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#solar-panel-installations</v>
+        <v>#pollutant-concentrations</v>
       </c>
       <c r="K85" s="7" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A86" s="8">
         <f t="shared" si="5"/>
         <v>83</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>316</v>
+        <v>301</v>
       </c>
       <c r="D86" s="10">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="E86" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G86" s="10" t="s">
-        <v>317</v>
+        <v>302</v>
+      </c>
+      <c r="G86" s="14" t="s">
+        <v>303</v>
       </c>
       <c r="H86" s="7" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
       <c r="I86" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>access-to-public-green-space</v>
+        <f t="shared" si="8"/>
+        <v>recycling-rates</v>
       </c>
       <c r="J86" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#access-to-public-green-space</v>
+        <v>#recycling-rates</v>
       </c>
       <c r="K86" s="7" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A87" s="8">
         <f t="shared" si="5"/>
         <v>84</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="D87" s="10">
-        <v>2018</v>
+        <v>2022</v>
       </c>
       <c r="E87" s="7" t="s">
-        <v>298</v>
-      </c>
-      <c r="G87" s="14" t="s">
-        <v>321</v>
+        <v>307</v>
+      </c>
+      <c r="G87" s="10" t="s">
+        <v>308</v>
       </c>
       <c r="H87" s="7" t="s">
-        <v>322</v>
+        <v>309</v>
       </c>
       <c r="I87" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>tree-canopy-cover</v>
+        <f t="shared" si="8"/>
+        <v>energy-performance-certificate-ratings</v>
       </c>
       <c r="J87" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#tree-canopy-cover</v>
+        <v>#energy-performance-certificate-ratings</v>
       </c>
       <c r="K87" s="7" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A88" s="8">
         <f t="shared" si="5"/>
         <v>85</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>324</v>
+        <v>311</v>
       </c>
       <c r="D88" s="10">
         <v>2021</v>
       </c>
       <c r="E88" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G88" s="14" t="s">
-        <v>17</v>
+        <v>292</v>
+      </c>
+      <c r="G88" s="10" t="s">
+        <v>312</v>
       </c>
       <c r="H88" s="7" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="I88" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>method-of-travel-to-work</v>
+        <f t="shared" si="8"/>
+        <v>solar-panel-installations</v>
       </c>
       <c r="J88" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#method-of-travel-to-work</v>
+        <v>#solar-panel-installations</v>
       </c>
       <c r="K88" s="7" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="89" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A89" s="8">
         <f t="shared" si="5"/>
         <v>86</v>
       </c>
+      <c r="B89" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="C89" s="9" t="s">
-        <v>327</v>
-      </c>
-      <c r="G89" s="14"/>
+        <v>315</v>
+      </c>
+      <c r="D89" s="10">
+        <v>2020</v>
+      </c>
+      <c r="E89" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G89" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="H89" s="7" t="s">
+        <v>317</v>
+      </c>
       <c r="I89" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>housing-and-infrastructure-introduction</v>
+        <f t="shared" si="8"/>
+        <v>access-to-public-green-space</v>
       </c>
       <c r="J89" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#housing-and-infrastructure-introduction</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+        <v>#access-to-public-green-space</v>
+      </c>
+      <c r="K89" s="7" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A90" s="8">
         <f t="shared" si="5"/>
         <v>87</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>328</v>
+        <v>290</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="D90" s="10">
-        <v>2021</v>
+        <v>2018</v>
       </c>
       <c r="E90" s="7" t="s">
-        <v>16</v>
+        <v>297</v>
       </c>
       <c r="G90" s="14" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="H90" s="7" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="I90" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>tenure-type</v>
+        <f t="shared" si="8"/>
+        <v>tree-canopy-cover</v>
       </c>
       <c r="J90" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#tenure-type</v>
+        <v>#tree-canopy-cover</v>
       </c>
       <c r="K90" s="7" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A91" s="8">
         <f t="shared" si="5"/>
         <v>88</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>328</v>
+        <v>290</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="D91" s="10">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="E91" s="7" t="s">
-        <v>308</v>
+        <v>16</v>
       </c>
       <c r="G91" s="14" t="s">
-        <v>334</v>
+        <v>17</v>
+      </c>
+      <c r="H91" s="7" t="s">
+        <v>324</v>
       </c>
       <c r="I91" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>dwelling-type</v>
+        <f t="shared" si="8"/>
+        <v>method-of-travel-to-work</v>
       </c>
       <c r="J91" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#dwelling-type</v>
+        <v>#method-of-travel-to-work</v>
       </c>
       <c r="K91" s="7" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A92" s="8">
         <f t="shared" si="5"/>
         <v>89</v>
       </c>
-      <c r="B92" s="7" t="s">
-        <v>328</v>
-      </c>
       <c r="C92" s="9" t="s">
-        <v>336</v>
-      </c>
-      <c r="D92" s="10">
-        <v>2022</v>
-      </c>
-      <c r="E92" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G92" s="14" t="s">
-        <v>337</v>
-      </c>
-      <c r="H92" s="7" t="s">
-        <v>338</v>
-      </c>
+        <v>326</v>
+      </c>
+      <c r="G92" s="14"/>
       <c r="I92" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>house-prices</v>
+        <f t="shared" si="8"/>
+        <v>housing-and-infrastructure-introduction</v>
       </c>
       <c r="J92" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#house-prices</v>
-      </c>
-      <c r="K92" s="7" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
+        <v>#housing-and-infrastructure-introduction</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A93" s="8">
         <f t="shared" si="5"/>
         <v>90</v>
       </c>
       <c r="B93" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="C93" s="9" t="s">
         <v>328</v>
-      </c>
-      <c r="C93" s="9" t="s">
-        <v>340</v>
       </c>
       <c r="D93" s="10">
         <v>2021</v>
@@ -4844,380 +4938,482 @@
       <c r="E93" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G93" s="10" t="s">
-        <v>341</v>
+      <c r="G93" s="14" t="s">
+        <v>329</v>
       </c>
       <c r="H93" s="7" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="I93" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>council-tax-bands</v>
+        <f t="shared" si="8"/>
+        <v>tenure-type</v>
       </c>
       <c r="J93" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#council-tax-bands</v>
+        <v>#tenure-type</v>
       </c>
       <c r="K93" s="7" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A94" s="8">
         <f t="shared" si="5"/>
         <v>91</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C94" s="9" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="D94" s="10">
-        <v>2015</v>
+        <v>2022</v>
       </c>
       <c r="E94" s="7" t="s">
-        <v>286</v>
-      </c>
-      <c r="G94" s="10" t="s">
-        <v>345</v>
+        <v>307</v>
+      </c>
+      <c r="G94" s="14" t="s">
+        <v>333</v>
       </c>
       <c r="I94" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>public-transport-accessibility</v>
+        <f t="shared" si="8"/>
+        <v>dwelling-type</v>
       </c>
       <c r="J94" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#public-transport-accessibility</v>
+        <v>#dwelling-type</v>
       </c>
       <c r="K94" s="7" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11" ht="87" x14ac:dyDescent="0.35">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A95" s="8">
         <f t="shared" si="5"/>
         <v>92</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
       <c r="D95" s="10">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="E95" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="G95" s="10" t="s">
-        <v>349</v>
+        <v>16</v>
+      </c>
+      <c r="G95" s="14" t="s">
+        <v>336</v>
       </c>
       <c r="H95" s="7" t="s">
-        <v>350</v>
+        <v>337</v>
       </c>
       <c r="I95" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>road-traffic</v>
+        <f t="shared" si="8"/>
+        <v>house-prices</v>
       </c>
       <c r="J95" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#road-traffic</v>
+        <v>#house-prices</v>
       </c>
       <c r="K95" s="7" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A96" s="8">
         <f t="shared" si="5"/>
         <v>93</v>
       </c>
+      <c r="B96" s="7" t="s">
+        <v>327</v>
+      </c>
       <c r="C96" s="9" t="s">
-        <v>352</v>
+        <v>339</v>
+      </c>
+      <c r="D96" s="10">
+        <v>2021</v>
+      </c>
+      <c r="E96" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G96" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="H96" s="7" t="s">
+        <v>341</v>
       </c>
       <c r="I96" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>community-introduction</v>
+        <f t="shared" si="8"/>
+        <v>council-tax-bands</v>
       </c>
       <c r="J96" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#community-introduction</v>
+        <v>#council-tax-bands</v>
       </c>
       <c r="K96" s="7" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="97" spans="1:13" ht="145" x14ac:dyDescent="0.35">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A97" s="8">
         <f t="shared" si="5"/>
         <v>94</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>353</v>
+        <v>327</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
       <c r="D97" s="10">
-        <v>2022</v>
+        <v>2015</v>
       </c>
       <c r="E97" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="G97" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="H97" s="7" t="s">
-        <v>355</v>
+        <v>285</v>
+      </c>
+      <c r="G97" s="10" t="s">
+        <v>344</v>
       </c>
       <c r="I97" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>resident-survey-results---overall-and-council</v>
+        <f t="shared" si="8"/>
+        <v>public-transport-accessibility</v>
       </c>
       <c r="J97" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#resident-survey-results---overall-and-council</v>
+        <v>#public-transport-accessibility</v>
       </c>
       <c r="K97" s="7" t="s">
-        <v>356</v>
-      </c>
-      <c r="M97" s="7"/>
-    </row>
-    <row r="98" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A98" s="8">
         <f t="shared" si="5"/>
         <v>95</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>353</v>
+        <v>327</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>357</v>
+        <v>346</v>
       </c>
       <c r="D98" s="10">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="E98" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="G98" s="14" t="s">
-        <v>358</v>
+        <v>347</v>
+      </c>
+      <c r="G98" s="10" t="s">
+        <v>348</v>
       </c>
       <c r="H98" s="7" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="I98" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>resident-survey-results---improving-the-area</v>
+        <f t="shared" si="8"/>
+        <v>road-traffic</v>
       </c>
       <c r="J98" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#resident-survey-results---improving-the-area</v>
+        <v>#road-traffic</v>
       </c>
       <c r="K98" s="7" t="s">
-        <v>360</v>
-      </c>
-      <c r="L98" s="7"/>
-    </row>
-    <row r="99" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A99" s="8">
         <f t="shared" si="5"/>
         <v>96</v>
       </c>
-      <c r="B99" s="7" t="s">
-        <v>353</v>
-      </c>
       <c r="C99" s="9" t="s">
-        <v>361</v>
-      </c>
-      <c r="D99" s="10">
-        <v>2022</v>
-      </c>
-      <c r="E99" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="G99" s="14" t="s">
-        <v>362</v>
-      </c>
-      <c r="H99" s="7" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="I99" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>resident-survey-results---local-area</v>
+        <f t="shared" si="8"/>
+        <v>community-introduction</v>
       </c>
       <c r="J99" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#resident-survey-results---local-area</v>
+        <v>#community-introduction</v>
       </c>
       <c r="K99" s="7" t="s">
-        <v>364</v>
-      </c>
-      <c r="L99" s="7"/>
-      <c r="M99" s="7"/>
-    </row>
-    <row r="100" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A100" s="8">
         <f t="shared" si="5"/>
         <v>97</v>
       </c>
       <c r="B100" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="C100" s="9" t="s">
         <v>353</v>
       </c>
-      <c r="C100" s="9" t="s">
-        <v>365</v>
-      </c>
       <c r="D100" s="10">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="E100" s="7" t="s">
-        <v>16</v>
+        <v>102</v>
       </c>
       <c r="G100" s="14" t="s">
-        <v>366</v>
+        <v>103</v>
       </c>
       <c r="H100" s="7" t="s">
-        <v>367</v>
+        <v>354</v>
       </c>
       <c r="I100" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>electoral-registration</v>
+        <f t="shared" si="8"/>
+        <v>resident-survey-results---overall-and-council</v>
       </c>
       <c r="J100" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#electoral-registration</v>
+        <v>#resident-survey-results---overall-and-council</v>
       </c>
       <c r="K100" s="7" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="101" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+        <v>355</v>
+      </c>
+      <c r="M100" s="7"/>
+    </row>
+    <row r="101" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A101" s="8">
         <f t="shared" si="5"/>
         <v>98</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="D101" s="10">
         <v>2022</v>
       </c>
       <c r="E101" s="7" t="s">
-        <v>370</v>
-      </c>
-      <c r="G101" s="10" t="s">
-        <v>371</v>
+        <v>102</v>
+      </c>
+      <c r="G101" s="14" t="s">
+        <v>357</v>
       </c>
       <c r="H101" s="7" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
       <c r="I101" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>local-election-turnout</v>
+        <f t="shared" si="8"/>
+        <v>resident-survey-results---improving-the-area</v>
       </c>
       <c r="J101" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#local-election-turnout</v>
+        <v>#resident-survey-results---improving-the-area</v>
       </c>
       <c r="K101" s="7" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="102" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+        <v>359</v>
+      </c>
+      <c r="L101" s="7"/>
+    </row>
+    <row r="102" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A102" s="8">
         <f t="shared" si="5"/>
         <v>99</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C102" s="9" t="s">
-        <v>374</v>
+        <v>360</v>
       </c>
       <c r="D102" s="10">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="E102" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G102" s="10" t="s">
-        <v>375</v>
+        <v>102</v>
+      </c>
+      <c r="G102" s="14" t="s">
+        <v>361</v>
       </c>
       <c r="H102" s="7" t="s">
-        <v>376</v>
+        <v>362</v>
       </c>
       <c r="I102" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>internet-users</v>
+        <f t="shared" si="8"/>
+        <v>resident-survey-results---local-area</v>
       </c>
       <c r="J102" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#internet-users</v>
+        <v>#resident-survey-results---local-area</v>
       </c>
       <c r="K102" s="7" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="103" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+        <v>363</v>
+      </c>
+      <c r="L102" s="7"/>
+      <c r="M102" s="7"/>
+    </row>
+    <row r="103" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A103" s="8">
         <f t="shared" si="5"/>
         <v>100</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C103" s="9" t="s">
-        <v>378</v>
+        <v>364</v>
       </c>
       <c r="D103" s="10">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="E103" s="7" t="s">
-        <v>102</v>
+        <v>16</v>
       </c>
       <c r="G103" s="14" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="H103" s="7" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="I103" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>internet-users---resident-survey</v>
+        <f t="shared" si="8"/>
+        <v>electoral-registration</v>
       </c>
       <c r="J103" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>#internet-users---resident-survey</v>
+        <v>#electoral-registration</v>
       </c>
       <c r="K103" s="7" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.35">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="8">
         <f t="shared" si="5"/>
         <v>101</v>
       </c>
+      <c r="B104" s="7" t="s">
+        <v>352</v>
+      </c>
       <c r="C104" s="9" t="s">
-        <v>380</v>
-      </c>
-      <c r="G104" s="14"/>
+        <v>368</v>
+      </c>
+      <c r="D104" s="10">
+        <v>2022</v>
+      </c>
+      <c r="E104" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="G104" s="10" t="s">
+        <v>370</v>
+      </c>
+      <c r="H104" s="7" t="s">
+        <v>371</v>
+      </c>
       <c r="I104" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
+        <v>local-election-turnout</v>
+      </c>
+      <c r="J104" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>#local-election-turnout</v>
+      </c>
+      <c r="K104" s="7" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A105" s="8">
+        <f t="shared" si="5"/>
+        <v>102</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="C105" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="D105" s="10">
+        <v>2020</v>
+      </c>
+      <c r="E105" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G105" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="H105" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="I105" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>internet-users</v>
+      </c>
+      <c r="J105" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>#internet-users</v>
+      </c>
+      <c r="K105" s="7" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A106" s="8">
+        <f t="shared" si="5"/>
+        <v>103</v>
+      </c>
+      <c r="B106" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="C106" s="9" t="s">
+        <v>377</v>
+      </c>
+      <c r="D106" s="10">
+        <v>2022</v>
+      </c>
+      <c r="E106" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="G106" s="14" t="s">
+        <v>361</v>
+      </c>
+      <c r="H106" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="I106" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>internet-users---resident-survey</v>
+      </c>
+      <c r="J106" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>#internet-users---resident-survey</v>
+      </c>
+      <c r="K106" s="7" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A107" s="8">
+        <f t="shared" si="5"/>
+        <v>104</v>
+      </c>
+      <c r="C107" s="9" t="s">
+        <v>379</v>
+      </c>
+      <c r="G107" s="14"/>
+      <c r="I107" s="7" t="str">
+        <f t="shared" si="8"/>
         <v>data-sources</v>
       </c>
-      <c r="J104" s="7" t="str">
+      <c r="J107" s="7" t="str">
         <f t="shared" si="4"/>
         <v>#data-sources</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="E105" s="10"/>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E108" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -5233,52 +5429,52 @@
     <hyperlink ref="G15" r:id="rId9" xr:uid="{6C31F9D7-263F-46D7-B63B-161FBD1E934D}"/>
     <hyperlink ref="G10" r:id="rId10" xr:uid="{9243BBAE-91D9-4291-89D5-20B3DA1C26E6}"/>
     <hyperlink ref="G9" r:id="rId11" xr:uid="{ADD359CE-3315-442E-B50D-5877AAD64B0D}"/>
-    <hyperlink ref="G88" r:id="rId12" xr:uid="{ED47DF1C-F425-4694-90E9-1FDFE85D42E0}"/>
+    <hyperlink ref="G91" r:id="rId12" xr:uid="{ED47DF1C-F425-4694-90E9-1FDFE85D42E0}"/>
     <hyperlink ref="G11" r:id="rId13" xr:uid="{5DFB4E02-9609-48D7-98DE-BEED2016CC9D}"/>
     <hyperlink ref="G8" r:id="rId14" xr:uid="{306009B9-67E9-42BF-A0E6-82F442B592F2}"/>
     <hyperlink ref="G24" r:id="rId15" xr:uid="{0DF09553-14C6-4217-88E3-F5245CA62B64}"/>
-    <hyperlink ref="G66" r:id="rId16" xr:uid="{00CEFB10-34B5-4BB2-B909-A0FF1E20D96A}"/>
-    <hyperlink ref="G67" r:id="rId17" xr:uid="{DDC1D92E-59B9-48D5-AB24-2231A32C15C4}"/>
-    <hyperlink ref="G71" r:id="rId18" xr:uid="{246ACD5F-29D0-4674-ABA7-62EB781D8DC8}"/>
-    <hyperlink ref="G83" r:id="rId19" xr:uid="{C89D75CA-4CB7-432F-9B31-1B81AC4F0707}"/>
-    <hyperlink ref="G87" r:id="rId20" xr:uid="{35867C5C-7BC8-470D-A8A2-1E30E3260E9B}"/>
+    <hyperlink ref="G69" r:id="rId16" xr:uid="{00CEFB10-34B5-4BB2-B909-A0FF1E20D96A}"/>
+    <hyperlink ref="G70" r:id="rId17" xr:uid="{DDC1D92E-59B9-48D5-AB24-2231A32C15C4}"/>
+    <hyperlink ref="G74" r:id="rId18" xr:uid="{246ACD5F-29D0-4674-ABA7-62EB781D8DC8}"/>
+    <hyperlink ref="G86" r:id="rId19" xr:uid="{C89D75CA-4CB7-432F-9B31-1B81AC4F0707}"/>
+    <hyperlink ref="G90" r:id="rId20" xr:uid="{35867C5C-7BC8-470D-A8A2-1E30E3260E9B}"/>
     <hyperlink ref="G12" r:id="rId21" xr:uid="{D2093666-A6DF-4FDE-A493-7B104DEAB349}"/>
     <hyperlink ref="G13" r:id="rId22" xr:uid="{B07705E2-4299-4D51-8751-BDF199E3708E}"/>
-    <hyperlink ref="G90" r:id="rId23" xr:uid="{91EF0389-E39A-483D-A49C-8723357272BD}"/>
-    <hyperlink ref="G76" r:id="rId24" xr:uid="{11D5CF9F-1854-4393-9CF6-0F7FCFAA5F8F}"/>
-    <hyperlink ref="G79" r:id="rId25" xr:uid="{1A6DE16B-98A5-4874-9CDD-6C38B28E269E}"/>
-    <hyperlink ref="G100" r:id="rId26" xr:uid="{75F090A1-59B0-4427-B568-781C58942D81}"/>
-    <hyperlink ref="G92" r:id="rId27" xr:uid="{ED6BF665-C78F-4B48-B3F6-F5FD4531826D}"/>
-    <hyperlink ref="G91" r:id="rId28" xr:uid="{90EB0F31-8C61-47E9-A55B-0BC257B5B05E}"/>
+    <hyperlink ref="G93" r:id="rId23" xr:uid="{91EF0389-E39A-483D-A49C-8723357272BD}"/>
+    <hyperlink ref="G79" r:id="rId24" xr:uid="{11D5CF9F-1854-4393-9CF6-0F7FCFAA5F8F}"/>
+    <hyperlink ref="G82" r:id="rId25" xr:uid="{1A6DE16B-98A5-4874-9CDD-6C38B28E269E}"/>
+    <hyperlink ref="G103" r:id="rId26" xr:uid="{75F090A1-59B0-4427-B568-781C58942D81}"/>
+    <hyperlink ref="G95" r:id="rId27" xr:uid="{ED6BF665-C78F-4B48-B3F6-F5FD4531826D}"/>
+    <hyperlink ref="G94" r:id="rId28" xr:uid="{90EB0F31-8C61-47E9-A55B-0BC257B5B05E}"/>
     <hyperlink ref="G21" r:id="rId29" xr:uid="{408D34C1-509E-40FC-BFEE-A463C4A4274B}"/>
-    <hyperlink ref="G70" r:id="rId30" xr:uid="{F51BDF5F-E5A3-4F0A-B3A8-74E2C5E73A9B}"/>
+    <hyperlink ref="G73" r:id="rId30" xr:uid="{F51BDF5F-E5A3-4F0A-B3A8-74E2C5E73A9B}"/>
     <hyperlink ref="G34" r:id="rId31" xr:uid="{C8ACE024-E7A1-4E66-BB37-A9E47655E075}"/>
     <hyperlink ref="G29" r:id="rId32" display="https://www.trustforlondon.org.uk/data/topics/living-standards/" xr:uid="{55918F9E-BDAC-4D36-B6B5-4A00416A4520}"/>
-    <hyperlink ref="F76" r:id="rId33" xr:uid="{C08426BD-102B-4D9D-9C29-86149025FA60}"/>
+    <hyperlink ref="F79" r:id="rId33" xr:uid="{C08426BD-102B-4D9D-9C29-86149025FA60}"/>
     <hyperlink ref="G50" r:id="rId34" xr:uid="{3D694CA2-9E9E-45C5-83BB-8BA3213AFADD}"/>
-    <hyperlink ref="G60" r:id="rId35" xr:uid="{D68C18A6-7527-4405-872E-E7F588CCE68B}"/>
+    <hyperlink ref="G63" r:id="rId35" xr:uid="{D68C18A6-7527-4405-872E-E7F588CCE68B}"/>
     <hyperlink ref="G49" r:id="rId36" xr:uid="{02115E8E-7C4D-44D8-B69A-8828B45B4551}"/>
-    <hyperlink ref="G59" r:id="rId37" location="page/4/gid/1000044/pat/6/ati/401/are/E09000022/iid/93721/age/163/sex/4/cat/-1/ctp/-1/yrr/1/cid/4/tbm/1" xr:uid="{DD1FDD19-586F-48C8-AA9A-A143808C6578}"/>
+    <hyperlink ref="G62" r:id="rId37" location="page/4/gid/1000044/pat/6/ati/401/are/E09000022/iid/93721/age/163/sex/4/cat/-1/ctp/-1/yrr/1/cid/4/tbm/1" xr:uid="{DD1FDD19-586F-48C8-AA9A-A143808C6578}"/>
     <hyperlink ref="G46" r:id="rId38" location="page/4/gid/8000011/pat/6/ati/402/are/E09000022/iid/20601/age/200/sex/4/cat/-1/ctp/-1/yrr/1/cid/4/tbm/1" xr:uid="{A8FABDE3-46B0-4F2F-8A3E-8C368DCE40AD}"/>
     <hyperlink ref="G47" r:id="rId39" location="page/4/gid/8000011/pat/6/ati/402/are/E09000022/iid/20602/age/201/sex/4/cat/-1/ctp/-1/yrr/1/cid/4/tbm/1" xr:uid="{C303BE21-35FE-4773-8CA5-DF1EB9A0C934}"/>
     <hyperlink ref="G48" r:id="rId40" location="page/4/gid/1938133258/pat/6/par/E12000007/ati/302/are/E09000022/iid/90631/age/34/sex/4/cat/-1/ctp/-1/yrr/1/cid/4/tbm/1/page-options/car-do-0" xr:uid="{054E050A-98AE-4EFF-86D9-7AD0683ACAC4}"/>
     <hyperlink ref="G51" r:id="rId41" location="page/4/gid/1/pat/6/par/E12000007/ati/402/are/E09000022/iid/91523/age/1/sex/4/cat/-1/ctp/-1/yrr/1/cid/4/tbm/1/page-options/car-do-0" xr:uid="{F4699B30-2FE0-49F4-A97F-2A80D1A3A237}"/>
     <hyperlink ref="G54" r:id="rId42" location="page/4/gid/1938132886/pat/6/par/E12000007/ati/402/are/E09000022/iid/91547/age/188/sex/4/cat/-1/ctp/-1/yrr/1/cid/4/tbm/1/page-options/car-do-0" xr:uid="{6C2015EF-2508-4B70-AD06-918B31212506}"/>
     <hyperlink ref="G55" r:id="rId43" location="page/4/gid/1938133001/pat/15/par/E92000001/ati/402/are/E09000022/iid/219/age/1/sex/4/cat/-1/ctp/-1/yrr/1/cid/4/tbm/1/page-options/car-do-0" xr:uid="{C4541972-CF60-4B66-972D-E475E40E42FF}"/>
-    <hyperlink ref="G58" r:id="rId44" location="page/4/gid/1000049/pat/6/par/E12000007/ati/102/are/E09000022/iid/90362/age/1/sex/1/cat/-1/ctp/-1/yrr/3/cid/4/tbm/1/page-options/car-do-0" xr:uid="{0CEF1DC8-5859-4668-B57E-7E5612FFD5B0}"/>
-    <hyperlink ref="G61" r:id="rId45" location="page/4/gid/1938133056/pat/6/par/E12000007/ati/402/are/E09000022/iid/93723/age/163/sex/4/cat/-1/ctp/-1/yrr/1/cid/4/tbm/1/page-options/car-do-0" xr:uid="{D7BB5F78-B652-4502-8C3B-7E2A52C70C39}"/>
-    <hyperlink ref="G62" r:id="rId46" location="page/4/gid/1938133056/pat/6/par/E12000007/ati/402/are/E09000022/iid/93722/age/163/sex/4/cat/-1/ctp/-1/yrr/1/cid/4/tbm/1/page-options/car-do-0" xr:uid="{E92A111C-B05E-4452-9233-6DCA36D23B28}"/>
-    <hyperlink ref="G63" r:id="rId47" location="page/4/gid/1938133056/pat/6/par/E12000007/ati/402/are/E09000022/iid/93720/age/163/sex/4/cat/-1/ctp/-1/yrr/1/cid/4/tbm/1/page-options/car-do-0" xr:uid="{C0627377-2432-4EAD-A7C8-73584BB31E38}"/>
-    <hyperlink ref="G64" r:id="rId48" location="page/4/gid/1938133056/pat/6/par/E12000007/ati/402/are/E09000022/iid/93724/age/163/sex/4/cat/-1/ctp/-1/yrr/1/cid/4/tbm/1/page-options/car-do-0" xr:uid="{14900D60-065A-41B0-B65E-05F0CDEA4096}"/>
+    <hyperlink ref="G61" r:id="rId44" location="page/4/gid/1000049/pat/6/par/E12000007/ati/102/are/E09000022/iid/90362/age/1/sex/1/cat/-1/ctp/-1/yrr/3/cid/4/tbm/1/page-options/car-do-0" xr:uid="{0CEF1DC8-5859-4668-B57E-7E5612FFD5B0}"/>
+    <hyperlink ref="G64" r:id="rId45" location="page/4/gid/1938133056/pat/6/par/E12000007/ati/402/are/E09000022/iid/93723/age/163/sex/4/cat/-1/ctp/-1/yrr/1/cid/4/tbm/1/page-options/car-do-0" xr:uid="{D7BB5F78-B652-4502-8C3B-7E2A52C70C39}"/>
+    <hyperlink ref="G65" r:id="rId46" location="page/4/gid/1938133056/pat/6/par/E12000007/ati/402/are/E09000022/iid/93722/age/163/sex/4/cat/-1/ctp/-1/yrr/1/cid/4/tbm/1/page-options/car-do-0" xr:uid="{E92A111C-B05E-4452-9233-6DCA36D23B28}"/>
+    <hyperlink ref="G66" r:id="rId47" location="page/4/gid/1938133056/pat/6/par/E12000007/ati/402/are/E09000022/iid/93720/age/163/sex/4/cat/-1/ctp/-1/yrr/1/cid/4/tbm/1/page-options/car-do-0" xr:uid="{C0627377-2432-4EAD-A7C8-73584BB31E38}"/>
+    <hyperlink ref="G67" r:id="rId48" location="page/4/gid/1938133056/pat/6/par/E12000007/ati/402/are/E09000022/iid/93724/age/163/sex/4/cat/-1/ctp/-1/yrr/1/cid/4/tbm/1/page-options/car-do-0" xr:uid="{14900D60-065A-41B0-B65E-05F0CDEA4096}"/>
     <hyperlink ref="G52" r:id="rId49" location="page/4/gid/1938132899/pat/15/par/E92000001/ati/402/are/E09000022/yrr/1/cid/4/tbm/1/page-options/car-do-0" xr:uid="{EEF27D22-987A-48E9-B508-9243B03B07F5}"/>
     <hyperlink ref="G53" r:id="rId50" location="page/4/gid/1938133001/pat/15/par/E92000001/ati/402/are/E09000022/iid/93088/age/168/sex/4/cat/-1/ctp/-1/yrr/1/cid/4/tbm/1/page-options/car-do-0" xr:uid="{404F02B2-DBF9-442E-924B-B5F4F806E20D}"/>
-    <hyperlink ref="G68" r:id="rId51" xr:uid="{39E3799A-FE90-4857-AD7B-DA20CEB85455}"/>
-    <hyperlink ref="G69" r:id="rId52" xr:uid="{5B7CE1FA-8C54-4FC3-B712-C908487B2CA7}"/>
-    <hyperlink ref="G72" r:id="rId53" xr:uid="{CEF01504-E838-4C7B-B040-1F015D01DC5E}"/>
-    <hyperlink ref="G73" r:id="rId54" xr:uid="{C82033C7-8D54-4727-B307-E0E3AAF5E3C7}"/>
+    <hyperlink ref="G71" r:id="rId51" xr:uid="{39E3799A-FE90-4857-AD7B-DA20CEB85455}"/>
+    <hyperlink ref="G72" r:id="rId52" xr:uid="{5B7CE1FA-8C54-4FC3-B712-C908487B2CA7}"/>
+    <hyperlink ref="G75" r:id="rId53" xr:uid="{CEF01504-E838-4C7B-B040-1F015D01DC5E}"/>
+    <hyperlink ref="G76" r:id="rId54" xr:uid="{C82033C7-8D54-4727-B307-E0E3AAF5E3C7}"/>
     <hyperlink ref="G45" r:id="rId55" location="page/4/gid/1/pat/6/par/E12000007/ati/402/are/E09000022/iid/30309/age/31/sex/4/cat/-1/ctp/-1/yrr/1/cid/4/tbm/1/page-options/car-do-0" xr:uid="{9C1F8B5E-AB86-4A4F-B8F7-E08FCA90EB13}"/>
-    <hyperlink ref="G81" r:id="rId56" xr:uid="{064865D0-4D12-4551-BE9D-291CCEBD6CBD}"/>
-    <hyperlink ref="G57" r:id="rId57" location="page/4/gid/1000049/pat/6/par/E12000007/ati/102/are/E09000022/iid/90366/age/1/sex/1/cat/-1/ctp/-1/yrr/1/cid/4/tbm/1/page-options/car-do-0 " xr:uid="{E959D4E6-9FF1-4A19-96D2-38AE792EEC7D}"/>
+    <hyperlink ref="G84" r:id="rId56" xr:uid="{064865D0-4D12-4551-BE9D-291CCEBD6CBD}"/>
+    <hyperlink ref="G60" r:id="rId57" location="page/4/gid/1000049/pat/6/par/E12000007/ati/102/are/E09000022/iid/90366/age/1/sex/1/cat/-1/ctp/-1/yrr/1/cid/4/tbm/1/page-options/car-do-0 " xr:uid="{E959D4E6-9FF1-4A19-96D2-38AE792EEC7D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId58"/>
@@ -5286,6 +5482,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001D21FA43D02C144A93636862C106D7E0" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b485cd096978ab29bebfa582ab2a5a42">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="36fa22c9-99b0-4d6c-b13f-c2885a394772" xmlns:ns3="f3dc68d1-c7e7-41c5-bc1e-27f8873ad3d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7600401377ffebbb162f8bf2186d2e5" ns2:_="" ns3:_="">
     <xsd:import namespace="36fa22c9-99b0-4d6c-b13f-c2885a394772"/>
@@ -5490,7 +5695,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="f3dc68d1-c7e7-41c5-bc1e-27f8873ad3d3" xsi:nil="true"/>
@@ -5501,16 +5706,15 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E75D4AB4-8999-470F-9F5F-BA8283E9C460}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C69BBBE4-1631-495B-B572-5694C5C5DECD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5529,7 +5733,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CB5E0B3-A367-47D0-BA78-E90229C3C6C9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -5538,12 +5742,4 @@
     <ds:schemaRef ds:uri="36fa22c9-99b0-4d6c-b13f-c2885a394772"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E75D4AB4-8999-470F-9F5F-BA8283E9C460}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated Cost of Living Data Pack
Added Low Income, changed 'Unemployment' tab to 'Work'
</commit_message>
<xml_diff>
--- a/scripts/Data sources.xlsx
+++ b/scripts/Data sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lambeth.sharepoint.com/sites/Data-Analytics-Insight-DataScienceTeam-Private/Shared Documents/Data Science Team - Private/Better Neighbourhoods Index/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1539" documentId="13_ncr:1_{770093B1-AED3-49DB-9954-741B278843BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71EF400C-626C-4C30-86E9-1B7FCC0127AB}"/>
+  <xr:revisionPtr revIDLastSave="1569" documentId="13_ncr:1_{770093B1-AED3-49DB-9954-741B278843BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8DE6DD90-F6B2-4436-9844-C74CE7EF58AD}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" tabRatio="470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="92">
   <si>
     <t>Number</t>
   </si>
@@ -236,66 +236,84 @@
     <t>The percentage of people aged 65+ who are on pension credit</t>
   </si>
   <si>
-    <t>This graph shows the percentage of people aged 65+ who were received pension credit in August 2022. This is used to indicate people of pension age who in poverty. A significantly higher percentage of over 64s in Lambeth (26.5%) received pension credit compared with London and England (17.5% and 11%).
+    <t>https://www.ons.gov.uk/peoplepopulationandcommunity/householdcharacteristics/homeinternetandsocialmediausage/bulletins/householdandresidentcharacteristicsenglandandwales/census2021</t>
+  </si>
+  <si>
+    <t>Data sources</t>
+  </si>
+  <si>
+    <t>Unemployment benefit claimants</t>
+  </si>
+  <si>
+    <t>Cost of living</t>
+  </si>
+  <si>
+    <t>Cost of living - Resident survey</t>
+  </si>
+  <si>
+    <t>Borough-wide responses to Cost of living questions from the latest annual Resident survey</t>
+  </si>
+  <si>
+    <t>These four graphs show the responses of Lambeth residents to cost of Cost of living-related questions (conducted in autumn 2022). Almost half of respondents reported that their financial circumstances got worse in the past year. About 27% of Lambeth residents think it will be at least fairly difficult to pay for food in the coming year, almost half expect it will be at least fairly difficult to pay for energy, and just under 40% expect it will be at least fairly difficult to pay for their rent/mortgage.</t>
+  </si>
+  <si>
+    <t>Fuel poverty</t>
+  </si>
+  <si>
+    <t>Fuel poverty at sub-regional levels</t>
+  </si>
+  <si>
+    <t>Deprivation according to categories defined in the 2021 Census</t>
+  </si>
+  <si>
+    <t>https://www.ons.gov.uk/datasets/TS011/editions/2021/versions/4/filter-outputs/076fcbc4-8f49-44cb-ac5d-9109f4986f92#variables</t>
+  </si>
+  <si>
+    <t>Deprivation map</t>
+  </si>
+  <si>
+    <t>Deprivation components</t>
+  </si>
+  <si>
+    <t>Poverty rates by borough, defined as 60% of median household income after housing costs, AHC. This indicator uses a 5 year pooled sample to the stated time period</t>
+  </si>
+  <si>
+    <t>https://www.gov.uk/government/statistics/children-in-low-income-families-local-area-statistics-2014-to-2022</t>
+  </si>
+  <si>
+    <t>https://www.gov.uk/government/statistics/sub-regional-fuel-poverty-data-2023-2021-data</t>
+  </si>
+  <si>
+    <t>DWP, endchildpoverty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This graph shows the percentage of children (aged 0-15) living in relative low-income households by borough and for London as a whole. Relative low income is defined as 60% of median household income before housing costs, BHC. In the latest data, Lambeth's prevalence is most recently at 18%, which is slightly lower than England (19%) and slightly higher than London (17%). There is a slight upwards trend for all three regions, and Lambeth and England have been higher than London. 
+When accounting for housing costs, the children in low-income households increases significantly across all three regions, nearly doubling for Lambeth (36%) and London (33%) in FYE 2022. The national rate increases to 29%. Due to sampling issues during 2021/22 related to the Covid-19 pandemic, additional caution may be required in interpreting these statistics. We further recommend particular caution in interpreting year-on-year changes in local areas, and advise focussing on longer-term trends when looking at change over time.  </t>
+  </si>
+  <si>
+    <t>https://endchildpoverty.org.uk/child-poverty/</t>
+  </si>
+  <si>
+    <t>The percentage of children living in relative low income households, defined as 60% of median household income befter housing costs (BHC) and after housing costs (AHC, calculated by endchildpoverty)</t>
+  </si>
+  <si>
+    <t>This graph shows the percentage of people aged 65+ who were received pension credit in August 2022. Note that this does not include those who are eligible but not receiving pension credit. This is used to indicate people of pension age who in poverty. A significantly higher percentage of over 64s in Lambeth (26.5%) received pension credit compared with London and England (17.5% and 11%).
 Percentages of over 64s who receive pension credit has been decreasing steadily for all areas since 2017. In this year, ~30% of Lambeth pensioners were receiving pension credit.</t>
   </si>
   <si>
-    <t>https://www.ons.gov.uk/peoplepopulationandcommunity/householdcharacteristics/homeinternetandsocialmediausage/bulletins/householdandresidentcharacteristicsenglandandwales/census2021</t>
-  </si>
-  <si>
-    <t>Data sources</t>
-  </si>
-  <si>
-    <t>Unemployment benefit claimants</t>
-  </si>
-  <si>
-    <t>Cost of living</t>
-  </si>
-  <si>
-    <t>Cost of living - Resident survey</t>
-  </si>
-  <si>
-    <t>Borough-wide responses to Cost of living questions from the latest annual Resident survey</t>
-  </si>
-  <si>
-    <t>These four graphs show the responses of Lambeth residents to cost of Cost of living-related questions (conducted in autumn 2022). Almost half of respondents reported that their financial circumstances got worse in the past year. About 27% of Lambeth residents think it will be at least fairly difficult to pay for food in the coming year, almost half expect it will be at least fairly difficult to pay for energy, and just under 40% expect it will be at least fairly difficult to pay for their rent/mortgage.</t>
-  </si>
-  <si>
-    <t>Fuel poverty</t>
-  </si>
-  <si>
-    <t>Fuel poverty at sub-regional levels</t>
-  </si>
-  <si>
-    <t>Unemployment</t>
-  </si>
-  <si>
-    <t>Deprivation according to categories defined in the 2021 Census</t>
-  </si>
-  <si>
-    <t>https://www.ons.gov.uk/datasets/TS011/editions/2021/versions/4/filter-outputs/076fcbc4-8f49-44cb-ac5d-9109f4986f92#variables</t>
-  </si>
-  <si>
-    <t>Deprivation map</t>
-  </si>
-  <si>
-    <t>Deprivation components</t>
-  </si>
-  <si>
-    <t>Poverty rates by borough, defined as 60% of median household income after housing costs, AHC. This indicator uses a 5 year pooled sample to the stated time period</t>
-  </si>
-  <si>
-    <t>https://www.gov.uk/government/statistics/children-in-low-income-families-local-area-statistics-2014-to-2022</t>
-  </si>
-  <si>
-    <t>https://www.gov.uk/government/statistics/sub-regional-fuel-poverty-data-2023-2021-data</t>
-  </si>
-  <si>
-    <t>The percentage of children living in relative low income households, defined as 60% of median household income befter housing costs (BHC) and after housing costs (AHC)</t>
-  </si>
-  <si>
-    <t>This graph shows the percentage of children (aged 0-15) living in relative low-income households by borough and for London as a whole. Relative low income is defined as 60% of median household income before housing costs, BHC. In the latest data, Lambeth's prevalence is most recently at 18%, which is slightly lower than England (19%) and slightly higher than London (17%). There is a slight upwards trend for all three regions, and Lambeth and England have been higher than London. 
-When accounting for housing costs, the children in low-income households increases significantly across all three regions, nearly doubling for Lambeth (36%) and London (33%) in FYE 2022. The national rate increases to 29%.</t>
+    <t>Work</t>
+  </si>
+  <si>
+    <t>https://data.london.gov.uk/dataset/earning-below-llw</t>
+  </si>
+  <si>
+    <t>Low Income</t>
+  </si>
+  <si>
+    <t>Percent of population living below living wage in 2022 (London living wage for Lambeth and London, UK living wage for rest of England)</t>
+  </si>
+  <si>
+    <t>The graph shows the percent of the population in Lambeth, London, and the rest of England (excluding London) who are living with an income below the living wage in 2022. Lambeth and London values are calculated with the London living wage (LLW) from the prior year while England's value is calculated with the UK living wage, which is lower than LLW. Lambeth has a higher proportion of its residents living in Low Income (18%) compared to both London (14%) and England (12%).</t>
   </si>
 </sst>
 </file>
@@ -679,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H5" zoomScale="78" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -771,10 +789,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D3" s="8">
         <v>2021</v>
@@ -784,10 +802,10 @@
       </c>
       <c r="F3" s="13"/>
       <c r="G3" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I3" s="8" t="str">
         <f t="shared" ref="I3" si="1">LOWER(SUBSTITUTE(C3," ","-"))</f>
@@ -806,10 +824,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D4" s="8">
         <v>2021</v>
@@ -818,13 +836,13 @@
         <v>15</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I4" s="8" t="str">
         <f t="shared" ref="I4" si="2">LOWER(SUBSTITUTE(C4," ","-"))</f>
@@ -843,7 +861,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>57</v>
@@ -858,7 +876,7 @@
         <v>59</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I5" s="6" t="str">
         <f t="shared" si="0"/>
@@ -872,12 +890,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="116" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A6" s="10">
         <v>3</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>61</v>
@@ -886,13 +904,16 @@
         <v>2022</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>62</v>
+        <v>82</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>84</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I6" s="6" t="str">
         <f t="shared" si="0"/>
@@ -903,16 +924,16 @@
         <v>#children-in-low-income-households</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="L6" s="6"/>
     </row>
-    <row r="7" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A7" s="10">
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>63</v>
@@ -938,7 +959,7 @@
         <v>#pension-credit</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
@@ -946,10 +967,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D8" s="9">
         <v>2021</v>
@@ -958,17 +979,17 @@
         <v>15</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I8" s="6" t="str">
         <f t="shared" ref="I8" si="6">LOWER(SUBSTITUTE(C8," ","-"))</f>
         <v>fuel-poverty</v>
       </c>
       <c r="J8" s="6" t="str">
-        <f t="shared" ref="J8:J21" si="7">_xlfn.CONCAT("#",I8)</f>
+        <f t="shared" ref="J8:J22" si="7">_xlfn.CONCAT("#",I8)</f>
         <v>#fuel-poverty</v>
       </c>
     </row>
@@ -977,10 +998,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>70</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>71</v>
       </c>
       <c r="D9" s="9">
         <v>2022</v>
@@ -992,10 +1013,10 @@
         <v>56</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I9" s="6" t="str">
-        <f t="shared" ref="I9:I21" si="8">LOWER(SUBSTITUTE(C9," ","-"))</f>
+        <f t="shared" ref="I9:I22" si="8">LOWER(SUBSTITUTE(C9," ","-"))</f>
         <v>cost-of-living---resident-survey</v>
       </c>
       <c r="J9" s="6" t="str">
@@ -1003,7 +1024,7 @@
         <v>#cost-of-living---resident-survey</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="130.5" x14ac:dyDescent="0.35">
@@ -1011,10 +1032,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D10" s="9">
         <v>2023</v>
@@ -1048,7 +1069,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>49</v>
@@ -1080,52 +1101,50 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A12" s="10">
         <v>9</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>14</v>
+        <v>89</v>
       </c>
       <c r="D12" s="9">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>15</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>16</v>
+        <v>88</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>17</v>
+        <v>90</v>
       </c>
       <c r="I12" s="6" t="str">
         <f t="shared" si="8"/>
-        <v>population</v>
+        <v>low-income</v>
       </c>
       <c r="J12" s="6" t="str">
         <f t="shared" si="7"/>
-        <v>#population</v>
+        <v>#low-income</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="L12" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A13" s="10">
+        <f>A12+1</f>
         <v>10</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D13" s="9">
         <v>2021</v>
@@ -1137,29 +1156,33 @@
         <v>16</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I13" s="6" t="str">
         <f t="shared" si="8"/>
-        <v>household-composition</v>
+        <v>population</v>
       </c>
       <c r="J13" s="6" t="str">
         <f t="shared" si="7"/>
-        <v>#household-composition</v>
+        <v>#population</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A14" s="10">
+        <f t="shared" ref="A14:A23" si="9">A13+1</f>
         <v>11</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D14" s="9">
         <v>2021</v>
@@ -1171,29 +1194,30 @@
         <v>16</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I14" s="6" t="str">
         <f t="shared" si="8"/>
-        <v>country-of-birth</v>
+        <v>household-composition</v>
       </c>
       <c r="J14" s="6" t="str">
         <f t="shared" si="7"/>
-        <v>#country-of-birth</v>
+        <v>#household-composition</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" s="10">
+        <f t="shared" si="9"/>
         <v>12</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D15" s="9">
         <v>2021</v>
@@ -1205,29 +1229,30 @@
         <v>16</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I15" s="6" t="str">
         <f t="shared" si="8"/>
-        <v>passports-held</v>
+        <v>country-of-birth</v>
       </c>
       <c r="J15" s="6" t="str">
         <f t="shared" si="7"/>
-        <v>#passports-held</v>
+        <v>#country-of-birth</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A16" s="10">
+        <f t="shared" si="9"/>
         <v>13</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D16" s="9">
         <v>2021</v>
@@ -1239,29 +1264,30 @@
         <v>16</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I16" s="6" t="str">
         <f t="shared" si="8"/>
-        <v>main-language</v>
+        <v>passports-held</v>
       </c>
       <c r="J16" s="6" t="str">
         <f t="shared" si="7"/>
-        <v>#main-language</v>
+        <v>#passports-held</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A17" s="10">
+        <f t="shared" si="9"/>
         <v>14</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D17" s="9">
         <v>2021</v>
@@ -1273,29 +1299,30 @@
         <v>16</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I17" s="6" t="str">
         <f t="shared" si="8"/>
-        <v>english-proficiency</v>
+        <v>main-language</v>
       </c>
       <c r="J17" s="6" t="str">
         <f t="shared" si="7"/>
-        <v>#english-proficiency</v>
+        <v>#main-language</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="87" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A18" s="10">
+        <f t="shared" si="9"/>
         <v>15</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D18" s="9">
         <v>2021</v>
@@ -1307,29 +1334,30 @@
         <v>16</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I18" s="6" t="str">
         <f t="shared" si="8"/>
-        <v>ethnicity</v>
+        <v>english-proficiency</v>
       </c>
       <c r="J18" s="6" t="str">
         <f t="shared" si="7"/>
-        <v>#ethnicity</v>
+        <v>#english-proficiency</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A19" s="10">
+        <f t="shared" si="9"/>
         <v>16</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D19" s="9">
         <v>2021</v>
@@ -1341,29 +1369,30 @@
         <v>16</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I19" s="6" t="str">
         <f t="shared" si="8"/>
-        <v>religion</v>
+        <v>ethnicity</v>
       </c>
       <c r="J19" s="6" t="str">
         <f t="shared" si="7"/>
-        <v>#religion</v>
+        <v>#ethnicity</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A20" s="10">
+        <f t="shared" si="9"/>
         <v>17</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D20" s="9">
         <v>2021</v>
@@ -1375,29 +1404,30 @@
         <v>16</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I20" s="6" t="str">
         <f t="shared" si="8"/>
-        <v>sexual-orientation</v>
+        <v>religion</v>
       </c>
       <c r="J20" s="6" t="str">
         <f t="shared" si="7"/>
-        <v>#sexual-orientation</v>
+        <v>#religion</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="116" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A21" s="10">
+        <f t="shared" si="9"/>
         <v>18</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D21" s="9">
         <v>2021</v>
@@ -1409,53 +1439,89 @@
         <v>16</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I21" s="6" t="str">
         <f t="shared" si="8"/>
-        <v>gender-identity</v>
+        <v>sexual-orientation</v>
       </c>
       <c r="J21" s="6" t="str">
         <f t="shared" si="7"/>
+        <v>#sexual-orientation</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="116" x14ac:dyDescent="0.35">
+      <c r="A22" s="10">
+        <f t="shared" si="9"/>
+        <v>19</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="9">
+        <v>2021</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I22" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>gender-identity</v>
+      </c>
+      <c r="J22" s="6" t="str">
+        <f t="shared" si="7"/>
         <v>#gender-identity</v>
       </c>
-      <c r="K21" s="6" t="s">
+      <c r="K22" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A22" s="10">
-        <v>19</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="G22" s="12"/>
-      <c r="I22" s="6" t="str">
-        <f t="shared" ref="I22" si="9">LOWER(SUBSTITUTE(C22," ","-"))</f>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23" s="10">
+        <f t="shared" si="9"/>
+        <v>20</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G23" s="12"/>
+      <c r="I23" s="6" t="str">
+        <f t="shared" ref="I23" si="10">LOWER(SUBSTITUTE(C23," ","-"))</f>
         <v>data-sources</v>
       </c>
-      <c r="J22" s="6" t="str">
-        <f t="shared" ref="J22" si="10">_xlfn.CONCAT("#",I22)</f>
+      <c r="J23" s="6" t="str">
+        <f t="shared" ref="J23" si="11">_xlfn.CONCAT("#",I23)</f>
         <v>#data-sources</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E23" s="9"/>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E24" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="G12" r:id="rId1" xr:uid="{351E22CE-AC3B-4FF7-A61E-45D15D65A16E}"/>
-    <hyperlink ref="G14" r:id="rId2" xr:uid="{4C61D3BB-2A6E-4812-9A19-978FFAEDB77E}"/>
-    <hyperlink ref="G15" r:id="rId3" xr:uid="{5BEA3353-6451-4304-87FF-72727D8F0322}"/>
-    <hyperlink ref="G13" r:id="rId4" xr:uid="{615BD21F-35C8-45A6-B3F8-434EC77EA86D}"/>
-    <hyperlink ref="G18" r:id="rId5" xr:uid="{9243BBAE-91D9-4291-89D5-20B3DA1C26E6}"/>
-    <hyperlink ref="G17" r:id="rId6" xr:uid="{ADD359CE-3315-442E-B50D-5877AAD64B0D}"/>
-    <hyperlink ref="G19" r:id="rId7" xr:uid="{5DFB4E02-9609-48D7-98DE-BEED2016CC9D}"/>
-    <hyperlink ref="G16" r:id="rId8" xr:uid="{306009B9-67E9-42BF-A0E6-82F442B592F2}"/>
-    <hyperlink ref="G20" r:id="rId9" xr:uid="{D2093666-A6DF-4FDE-A493-7B104DEAB349}"/>
-    <hyperlink ref="G21" r:id="rId10" xr:uid="{B07705E2-4299-4D51-8751-BDF199E3708E}"/>
+    <hyperlink ref="G13" r:id="rId1" xr:uid="{351E22CE-AC3B-4FF7-A61E-45D15D65A16E}"/>
+    <hyperlink ref="G15" r:id="rId2" xr:uid="{4C61D3BB-2A6E-4812-9A19-978FFAEDB77E}"/>
+    <hyperlink ref="G16" r:id="rId3" xr:uid="{5BEA3353-6451-4304-87FF-72727D8F0322}"/>
+    <hyperlink ref="G14" r:id="rId4" xr:uid="{615BD21F-35C8-45A6-B3F8-434EC77EA86D}"/>
+    <hyperlink ref="G19" r:id="rId5" xr:uid="{9243BBAE-91D9-4291-89D5-20B3DA1C26E6}"/>
+    <hyperlink ref="G18" r:id="rId6" xr:uid="{ADD359CE-3315-442E-B50D-5877AAD64B0D}"/>
+    <hyperlink ref="G20" r:id="rId7" xr:uid="{5DFB4E02-9609-48D7-98DE-BEED2016CC9D}"/>
+    <hyperlink ref="G17" r:id="rId8" xr:uid="{306009B9-67E9-42BF-A0E6-82F442B592F2}"/>
+    <hyperlink ref="G21" r:id="rId9" xr:uid="{D2093666-A6DF-4FDE-A493-7B104DEAB349}"/>
+    <hyperlink ref="G22" r:id="rId10" xr:uid="{B07705E2-4299-4D51-8751-BDF199E3708E}"/>
     <hyperlink ref="G5" r:id="rId11" display="https://www.trustforlondon.org.uk/data/topics/living-standards/" xr:uid="{55918F9E-BDAC-4D36-B6B5-4A00416A4520}"/>
     <hyperlink ref="G10" r:id="rId12" xr:uid="{6E19827B-1BF5-4706-9357-BB9BA6EE32C8}"/>
     <hyperlink ref="G3" r:id="rId13" location="variables" xr:uid="{C4A7F7A1-6DB0-4126-B380-8CA24832F1ED}"/>
@@ -1463,9 +1529,10 @@
     <hyperlink ref="G6" r:id="rId15" xr:uid="{43613E11-CC69-4919-8E03-07A2F97DDA82}"/>
     <hyperlink ref="G7" r:id="rId16" xr:uid="{94E62556-CBED-47D9-A2D7-A5D2DBB4ACEE}"/>
     <hyperlink ref="G9" r:id="rId17" xr:uid="{874E092B-4FCC-430D-8491-9172E1B46607}"/>
+    <hyperlink ref="G8" r:id="rId18" xr:uid="{A8257AA2-32B6-47EC-86D0-33BAC67C99F2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId18"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated Cost of Living Fuel Poverty section
Added commentary and updated ward/LSOA data from 2020 to 2021
</commit_message>
<xml_diff>
--- a/scripts/Data sources.xlsx
+++ b/scripts/Data sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lambeth.sharepoint.com/sites/Data-Analytics-Insight-DataScienceTeam-Private/Shared Documents/Data Science Team - Private/Better Neighbourhoods Index/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1569" documentId="13_ncr:1_{770093B1-AED3-49DB-9954-741B278843BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8DE6DD90-F6B2-4436-9844-C74CE7EF58AD}"/>
+  <xr:revisionPtr revIDLastSave="1575" documentId="13_ncr:1_{770093B1-AED3-49DB-9954-741B278843BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0FD3B055-3CBB-41ED-B813-0D0B1AB027AE}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" tabRatio="470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="93">
   <si>
     <t>Number</t>
   </si>
@@ -314,6 +314,9 @@
   </si>
   <si>
     <t>The graph shows the percent of the population in Lambeth, London, and the rest of England (excluding London) who are living with an income below the living wage in 2022. Lambeth and London values are calculated with the London living wage (LLW) from the prior year while England's value is calculated with the UK living wage, which is lower than LLW. Lambeth has a higher proportion of its residents living in Low Income (18%) compared to both London (14%) and England (12%).</t>
+  </si>
+  <si>
+    <t>This graph shows the percentage of households living in fuel poverty, which is measured using the Low Income Low Energy Efficiency (LILEE) indicator. A household is considered to be fuel poor if they are living in a property with a fuel poverty energy efficiency rating of band D or below and when they spend the required amount to heat their home, they are left with a residual income below the official poverty line. Lambeth has a lower proportion (11%) in fuel poverty compared to London (12%) and England (13%). At the ward level, Streatham South has the highest proportion in fuel poverty (14%) while Clapham Common has the lowest (8%). Note that at the LSOA level, two were missing in the 2021 data (Lambeth 003E and Lambeth 004F).</t>
   </si>
 </sst>
 </file>
@@ -699,8 +702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="H6" zoomScale="78" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -991,6 +994,9 @@
       <c r="J8" s="6" t="str">
         <f t="shared" ref="J8:J22" si="7">_xlfn.CONCAT("#",I8)</f>
         <v>#fuel-poverty</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
@@ -1537,6 +1543,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="3762e1dc-9bcc-4a22-91e6-a5cb4b094858" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b7e4309d-338c-4222-aec5-3c776822f99d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E63038107AB36B45A5DA02DFD8E05274" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d662b2c0bcca501ec484ddb2c2692511">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b7e4309d-338c-4222-aec5-3c776822f99d" xmlns:ns3="9f317655-23b1-4c1f-850c-71f5c663da67" xmlns:ns4="3762e1dc-9bcc-4a22-91e6-a5cb4b094858" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d29307f3ded143c6e731bb4f79d88fd4" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="b7e4309d-338c-4222-aec5-3c776822f99d"/>
@@ -1784,42 +1810,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="3762e1dc-9bcc-4a22-91e6-a5cb4b094858" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b7e4309d-338c-4222-aec5-3c776822f99d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8110B3EE-04CD-4D80-A23D-024AD29EEA78}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E75D4AB4-8999-470F-9F5F-BA8283E9C460}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b7e4309d-338c-4222-aec5-3c776822f99d"/>
-    <ds:schemaRef ds:uri="9f317655-23b1-4c1f-850c-71f5c663da67"/>
-    <ds:schemaRef ds:uri="3762e1dc-9bcc-4a22-91e6-a5cb4b094858"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1843,9 +1837,21 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E75D4AB4-8999-470F-9F5F-BA8283E9C460}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8110B3EE-04CD-4D80-A23D-024AD29EEA78}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b7e4309d-338c-4222-aec5-3c776822f99d"/>
+    <ds:schemaRef ds:uri="9f317655-23b1-4c1f-850c-71f5c663da67"/>
+    <ds:schemaRef ds:uri="3762e1dc-9bcc-4a22-91e6-a5cb4b094858"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>